<commit_message>
added some of the first sequence diagrams
</commit_message>
<xml_diff>
--- a/Planning Report/application sprint planner sprint1 02.12.19.xlsx
+++ b/Planning Report/application sprint planner sprint1 02.12.19.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB05F862-0959-457D-A94C-2C4040583967}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151D3E45-89D7-4855-97AE-2E376B224B36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29130" yWindow="690" windowWidth="28200" windowHeight="14085" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22395" windowHeight="12030" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <definedName name="Today" localSheetId="0">TODAY()</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1412,6 +1413,40 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="92">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2917,40 +2952,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -3272,10 +3273,10 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="79"/>
-    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" dataCellStyle="Comma [0]"/>
@@ -3555,8 +3556,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BM119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="E43" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13195,9 +13196,15 @@
       <c r="E50" s="34">
         <v>6</v>
       </c>
-      <c r="F50" s="31"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="33"/>
+      <c r="F50" s="31">
+        <v>1</v>
+      </c>
+      <c r="G50" s="32">
+        <v>43808</v>
+      </c>
+      <c r="H50" s="33">
+        <v>1</v>
+      </c>
       <c r="I50" s="26"/>
       <c r="J50" s="38" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -27095,56 +27102,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:BM8 J116:BM117 J88:BM91 J97:BM97 J72:BM73 J94:BM94 J103:BM103 J83:BM86 J75:BM76 J10:BM10 J62:BM69 J22:BM59">
-    <cfRule type="expression" dxfId="75" priority="247">
+    <cfRule type="expression" dxfId="79" priority="247">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:AN4">
-    <cfRule type="expression" dxfId="74" priority="253">
+    <cfRule type="expression" dxfId="78" priority="253">
       <formula>J$5&lt;=EOMONTH($J$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:BM4">
-    <cfRule type="expression" dxfId="73" priority="249">
+    <cfRule type="expression" dxfId="77" priority="249">
       <formula>AND(K$5&lt;=EOMONTH($J$5,2),K$5&gt;EOMONTH($J$5,0),K$5&gt;EOMONTH($J$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BM4">
-    <cfRule type="expression" dxfId="72" priority="248">
+    <cfRule type="expression" dxfId="76" priority="248">
       <formula>AND(J$5&lt;=EOMONTH($J$5,1),J$5&gt;EOMONTH($J$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:BM8 J10:BM10 J22:BM116">
-    <cfRule type="expression" dxfId="71" priority="270" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="270" stopIfTrue="1">
       <formula>AND($D8="Low risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="289" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="289" stopIfTrue="1">
       <formula>AND($D8="High risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="307" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="307" stopIfTrue="1">
       <formula>AND($D8="On track",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="308" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="308" stopIfTrue="1">
       <formula>AND($D8="Med risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="309" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="309" stopIfTrue="1">
       <formula>AND(LEN($D8)=0,J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J117:BM117">
-    <cfRule type="expression" dxfId="66" priority="317" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="317" stopIfTrue="1">
       <formula>AND(#REF!="Low risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="318" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="318" stopIfTrue="1">
       <formula>AND(#REF!="High risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="319" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="319" stopIfTrue="1">
       <formula>AND(#REF!="On track",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="320" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="320" stopIfTrue="1">
       <formula>AND(#REF!="Med risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="321" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="321" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27163,24 +27170,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="61" priority="238">
+    <cfRule type="expression" dxfId="65" priority="238">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="60" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="240" stopIfTrue="1">
       <formula>AND($D9="Low risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="241" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="241" stopIfTrue="1">
       <formula>AND($D9="High risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="242" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="242" stopIfTrue="1">
       <formula>AND($D9="On track",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="243" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="243" stopIfTrue="1">
       <formula>AND($D9="Med risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="244" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="244" stopIfTrue="1">
       <formula>AND(LEN($D9)=0,J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27199,7 +27206,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J80:BM80 J77:BM78">
-    <cfRule type="expression" dxfId="55" priority="222">
+    <cfRule type="expression" dxfId="59" priority="222">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27218,7 +27225,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J82:GC82">
-    <cfRule type="expression" dxfId="54" priority="213">
+    <cfRule type="expression" dxfId="58" priority="213">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27237,7 +27244,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:BM81 J79:BM79">
-    <cfRule type="expression" dxfId="53" priority="206">
+    <cfRule type="expression" dxfId="57" priority="206">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27256,7 +27263,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J60:BM61">
-    <cfRule type="expression" dxfId="52" priority="198">
+    <cfRule type="expression" dxfId="56" priority="198">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27275,7 +27282,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87:GC87">
-    <cfRule type="expression" dxfId="51" priority="189">
+    <cfRule type="expression" dxfId="55" priority="189">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27294,7 +27301,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J98:GC99 J101:GC103 J106:GC106 J113:GC115">
-    <cfRule type="expression" dxfId="50" priority="182">
+    <cfRule type="expression" dxfId="54" priority="182">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27313,7 +27320,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:GC100">
-    <cfRule type="expression" dxfId="49" priority="174">
+    <cfRule type="expression" dxfId="53" priority="174">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27332,7 +27339,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J96:GC96">
-    <cfRule type="expression" dxfId="48" priority="165">
+    <cfRule type="expression" dxfId="52" priority="165">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27351,7 +27358,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J71:GC71">
-    <cfRule type="expression" dxfId="47" priority="157">
+    <cfRule type="expression" dxfId="51" priority="157">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27370,7 +27377,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J93:BM93">
-    <cfRule type="expression" dxfId="46" priority="149">
+    <cfRule type="expression" dxfId="50" priority="149">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27389,7 +27396,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J104:GC105">
-    <cfRule type="expression" dxfId="45" priority="141">
+    <cfRule type="expression" dxfId="49" priority="141">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27408,7 +27415,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J107:GC108">
-    <cfRule type="expression" dxfId="44" priority="133">
+    <cfRule type="expression" dxfId="48" priority="133">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27427,7 +27434,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J111:GC111">
-    <cfRule type="expression" dxfId="43" priority="125">
+    <cfRule type="expression" dxfId="47" priority="125">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27446,7 +27453,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J112:GC112">
-    <cfRule type="expression" dxfId="42" priority="117">
+    <cfRule type="expression" dxfId="46" priority="117">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27465,7 +27472,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J95:BM95">
-    <cfRule type="expression" dxfId="41" priority="109">
+    <cfRule type="expression" dxfId="45" priority="109">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27484,7 +27491,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J74:BM74">
-    <cfRule type="expression" dxfId="40" priority="101">
+    <cfRule type="expression" dxfId="44" priority="101">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27503,7 +27510,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J110:BM110">
-    <cfRule type="expression" dxfId="39" priority="93">
+    <cfRule type="expression" dxfId="43" priority="93">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27522,7 +27529,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J92:BM92">
-    <cfRule type="expression" dxfId="38" priority="61">
+    <cfRule type="expression" dxfId="42" priority="61">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27541,12 +27548,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:GC109">
-    <cfRule type="expression" dxfId="37" priority="69">
+    <cfRule type="expression" dxfId="41" priority="69">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70:BM70">
-    <cfRule type="expression" dxfId="36" priority="53">
+    <cfRule type="expression" dxfId="40" priority="53">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27579,24 +27586,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="35" priority="45">
+    <cfRule type="expression" dxfId="39" priority="45">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="34" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="47" stopIfTrue="1">
       <formula>AND($D11="Low risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="48" stopIfTrue="1">
       <formula>AND($D11="High risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="49" stopIfTrue="1">
       <formula>AND($D11="On track",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="50" stopIfTrue="1">
       <formula>AND($D11="Med risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="51" stopIfTrue="1">
       <formula>AND(LEN($D11)=0,J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27615,24 +27622,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="29" priority="37">
+    <cfRule type="expression" dxfId="33" priority="37">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="28" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="39" stopIfTrue="1">
       <formula>AND($D12="Low risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="40" stopIfTrue="1">
       <formula>AND($D12="High risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="41" stopIfTrue="1">
       <formula>AND($D12="On track",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="42" stopIfTrue="1">
       <formula>AND($D12="Med risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="43" stopIfTrue="1">
       <formula>AND(LEN($D12)=0,J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27651,24 +27658,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="23" priority="29">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="22" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="31" stopIfTrue="1">
       <formula>AND($D15="Low risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="32" stopIfTrue="1">
       <formula>AND($D15="High risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="33" stopIfTrue="1">
       <formula>AND($D15="On track",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="34" stopIfTrue="1">
       <formula>AND($D15="Med risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="35" stopIfTrue="1">
       <formula>AND(LEN($D15)=0,J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27687,46 +27694,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="21" priority="21">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="16" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
       <formula>AND($D16="Low risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="24" stopIfTrue="1">
       <formula>AND($D16="High risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="25" stopIfTrue="1">
       <formula>AND($D16="On track",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="26" stopIfTrue="1">
       <formula>AND($D16="Med risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="27" stopIfTrue="1">
       <formula>AND(LEN($D16)=0,J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="11" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
       <formula>AND($D19="Low risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
       <formula>AND($D19="High risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="18" stopIfTrue="1">
       <formula>AND($D19="On track",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="19" stopIfTrue="1">
       <formula>AND($D19="Med risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
       <formula>AND(LEN($D19)=0,J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="6" priority="13">
+    <cfRule type="expression" dxfId="10" priority="13">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27745,19 +27752,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:BM21">
-    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
       <formula>AND($D20="Low risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>AND($D20="High risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
       <formula>AND($D20="On track",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="11" stopIfTrue="1">
       <formula>AND($D20="Med risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="12" stopIfTrue="1">
       <formula>AND(LEN($D20)=0,J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27776,7 +27783,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:GC21">
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28319,6 +28326,51 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>F44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F2A40D55-1216-4905-A2E5-7E4EA7162C87}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F52</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BDF1EDAE-75A8-4A38-9730-5006E07D0D5D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F49</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{DB5DC438-E855-400C-8FB0-BE37FFB333E9}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="316" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
@@ -28871,51 +28923,6 @@
           </x14:cfRule>
           <xm:sqref>J20:BM21</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F2A40D55-1216-4905-A2E5-7E4EA7162C87}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F52</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BDF1EDAE-75A8-4A38-9730-5006E07D0D5D}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{DB5DC438-E855-400C-8FB0-BE37FFB333E9}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F47</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
UX fixes for allowing the survey, first draft of questionair, bug fix for user login skills creation
</commit_message>
<xml_diff>
--- a/Planning Report/application sprint planner sprint1 02.12.19.xlsx
+++ b/Planning Report/application sprint planner sprint1 02.12.19.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151D3E45-89D7-4855-97AE-2E376B224B36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBC3E5E-B3C7-40E3-9A35-C70FBA8DD9D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22395" windowHeight="12030" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6975" yWindow="1095" windowWidth="22395" windowHeight="12030" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <definedName name="Today" localSheetId="0">TODAY()</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="105">
   <si>
     <t>Create a Gantt Chart in this worksheet.
 Enter title of this project in cell B1. 
@@ -1413,40 +1412,6 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="92">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2952,6 +2917,40 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -3273,10 +3272,10 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="76"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" dataCellStyle="Comma [0]"/>
@@ -3556,8 +3555,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BM119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="E43" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="L66" sqref="L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11979,13 +11978,21 @@
         <v>90</v>
       </c>
       <c r="C45" s="53"/>
-      <c r="D45" s="34"/>
+      <c r="D45" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="E45" s="34">
         <v>4</v>
       </c>
-      <c r="F45" s="31"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="33"/>
+      <c r="F45" s="31">
+        <v>1</v>
+      </c>
+      <c r="G45" s="32">
+        <v>43810</v>
+      </c>
+      <c r="H45" s="33">
+        <v>2</v>
+      </c>
       <c r="I45" s="26"/>
       <c r="J45" s="38" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -12218,16 +12225,24 @@
         <v>91</v>
       </c>
       <c r="C46" s="53"/>
-      <c r="D46" s="34"/>
+      <c r="D46" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="E46" s="34">
         <v>4</v>
       </c>
-      <c r="F46" s="31"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="33"/>
+      <c r="F46" s="31">
+        <v>1</v>
+      </c>
+      <c r="G46" s="32">
+        <v>43810</v>
+      </c>
+      <c r="H46" s="33">
+        <v>2</v>
+      </c>
       <c r="I46" s="26"/>
       <c r="J46" s="38" t="str">
-        <f t="shared" ref="J46:AO52" ca="1" si="22">IF(AND($D46="Goal",J$5&gt;=$G46,J$5&lt;=$G46+$H46-1),2,IF(AND($D46="Milestone",J$5&gt;=$G46,J$5&lt;=$G46+$H46-1),1,""))</f>
+        <f t="shared" ref="J46:AO51" ca="1" si="22">IF(AND($D46="Goal",J$5&gt;=$G46,J$5&lt;=$G46+$H46-1),2,IF(AND($D46="Milestone",J$5&gt;=$G46,J$5&lt;=$G46+$H46-1),1,""))</f>
         <v/>
       </c>
       <c r="K46" s="38" t="str">
@@ -12701,16 +12716,24 @@
     <row r="48" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="B48" s="41" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="C48" s="53"/>
-      <c r="D48" s="34"/>
+      <c r="D48" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="E48" s="34">
         <v>2</v>
       </c>
-      <c r="F48" s="31"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="33"/>
+      <c r="F48" s="31">
+        <v>1</v>
+      </c>
+      <c r="G48" s="32">
+        <v>43803</v>
+      </c>
+      <c r="H48" s="33">
+        <v>1</v>
+      </c>
       <c r="I48" s="26"/>
       <c r="J48" s="38" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -12841,7 +12864,7 @@
         <v/>
       </c>
       <c r="AP48" s="38" t="str">
-        <f t="shared" ref="AP48:BE59" ca="1" si="23">IF(AND($D48="Goal",AP$5&gt;=$G48,AP$5&lt;=$G48+$H48-1),2,IF(AND($D48="Milestone",AP$5&gt;=$G48,AP$5&lt;=$G48+$H48-1),1,""))</f>
+        <f t="shared" ref="AP48:BE58" ca="1" si="23">IF(AND($D48="Goal",AP$5&gt;=$G48,AP$5&lt;=$G48+$H48-1),2,IF(AND($D48="Milestone",AP$5&gt;=$G48,AP$5&lt;=$G48+$H48-1),1,""))</f>
         <v/>
       </c>
       <c r="AQ48" s="38" t="str">
@@ -12905,7 +12928,7 @@
         <v/>
       </c>
       <c r="BF48" s="38" t="str">
-        <f t="shared" ref="BF48:BM59" ca="1" si="24">IF(AND($D48="Goal",BF$5&gt;=$G48,BF$5&lt;=$G48+$H48-1),2,IF(AND($D48="Milestone",BF$5&gt;=$G48,BF$5&lt;=$G48+$H48-1),1,""))</f>
+        <f t="shared" ref="BF48:BM58" ca="1" si="24">IF(AND($D48="Goal",BF$5&gt;=$G48,BF$5&lt;=$G48+$H48-1),2,IF(AND($D48="Milestone",BF$5&gt;=$G48,BF$5&lt;=$G48+$H48-1),1,""))</f>
         <v/>
       </c>
       <c r="BG48" s="38" t="str">
@@ -12940,20 +12963,20 @@
     <row r="49" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="41" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C49" s="53"/>
       <c r="D49" s="34" t="s">
         <v>17</v>
       </c>
       <c r="E49" s="34">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F49" s="31">
         <v>1</v>
       </c>
       <c r="G49" s="32">
-        <v>43803</v>
+        <v>43808</v>
       </c>
       <c r="H49" s="33">
         <v>1</v>
@@ -13187,20 +13210,20 @@
     <row r="50" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="41" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C50" s="53"/>
       <c r="D50" s="34" t="s">
         <v>17</v>
       </c>
       <c r="E50" s="34">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F50" s="31">
         <v>1</v>
       </c>
       <c r="G50" s="32">
-        <v>43808</v>
+        <v>43803</v>
       </c>
       <c r="H50" s="33">
         <v>1</v>
@@ -13434,14 +13457,14 @@
     <row r="51" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="41" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C51" s="53"/>
       <c r="D51" s="34" t="s">
         <v>17</v>
       </c>
       <c r="E51" s="34">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F51" s="31">
         <v>1</v>
@@ -13578,7 +13601,7 @@
         <v/>
       </c>
       <c r="AO51" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ref="J51:AO58" ca="1" si="25">IF(AND($D51="Goal",AO$5&gt;=$G51,AO$5&lt;=$G51+$H51-1),2,IF(AND($D51="Milestone",AO$5&gt;=$G51,AO$5&lt;=$G51+$H51-1),1,""))</f>
         <v/>
       </c>
       <c r="AP51" s="38" t="str">
@@ -13681,151 +13704,151 @@
     <row r="52" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="41" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="C52" s="53"/>
       <c r="D52" s="34" t="s">
         <v>17</v>
       </c>
       <c r="E52" s="34">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F52" s="31">
         <v>1</v>
       </c>
       <c r="G52" s="32">
-        <v>43803</v>
+        <v>43813</v>
       </c>
       <c r="H52" s="33">
         <v>1</v>
       </c>
       <c r="I52" s="26"/>
       <c r="J52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="K52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="L52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="M52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="N52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="O52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="P52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="Q52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="R52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="S52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="T52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="U52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="V52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="W52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="X52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="Y52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="Z52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AA52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AB52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AC52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AD52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AE52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AF52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AG52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AH52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AI52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AJ52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AK52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AL52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AM52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AN52" s="38" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AO52" s="38" t="str">
-        <f t="shared" ref="J52:AO59" ca="1" si="25">IF(AND($D52="Goal",AO$5&gt;=$G52,AO$5&lt;=$G52+$H52-1),2,IF(AND($D52="Milestone",AO$5&gt;=$G52,AO$5&lt;=$G52+$H52-1),1,""))</f>
+        <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
       <c r="AP52" s="38" t="str">
@@ -13928,16 +13951,20 @@
     <row r="53" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="41" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C53" s="53"/>
       <c r="D53" s="34"/>
       <c r="E53" s="34">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="F53" s="31"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="33"/>
+      <c r="G53" s="32">
+        <v>43809</v>
+      </c>
+      <c r="H53" s="33">
+        <v>1</v>
+      </c>
       <c r="I53" s="26"/>
       <c r="J53" s="38" t="str">
         <f t="shared" ca="1" si="25"/>
@@ -14405,14 +14432,10 @@
     </row>
     <row r="55" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
-      <c r="B55" s="41" t="s">
-        <v>67</v>
-      </c>
+      <c r="B55" s="53"/>
       <c r="C55" s="53"/>
       <c r="D55" s="34"/>
-      <c r="E55" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="E55" s="34"/>
       <c r="F55" s="31"/>
       <c r="G55" s="32"/>
       <c r="H55" s="33"/>
@@ -15347,9 +15370,9 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="53"/>
+    <row r="59" spans="1:65" s="2" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="15"/>
+      <c r="B59" s="41"/>
       <c r="C59" s="53"/>
       <c r="D59" s="34"/>
       <c r="E59" s="34"/>
@@ -15357,232 +15380,64 @@
       <c r="G59" s="32"/>
       <c r="H59" s="33"/>
       <c r="I59" s="26"/>
-      <c r="J59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="K59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="L59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="M59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="N59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="O59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="P59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Q59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="R59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="S59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="T59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="U59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="V59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="W59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="X59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Y59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Z59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AA59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AB59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AC59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AD59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AE59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AF59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AG59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AH59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AI59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AJ59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AK59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AL59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AM59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AN59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AO59" s="38" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AP59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AQ59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AR59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AS59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AT59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AU59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AV59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AW59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AX59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AY59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="AZ59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BA59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BB59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BC59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BD59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BE59" s="38" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BF59" s="38" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="BG59" s="38" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="BH59" s="38" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="BI59" s="38" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="BJ59" s="38" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="BK59" s="38" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="BL59" s="38" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="BM59" s="38" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
+      <c r="J59" s="38"/>
+      <c r="K59" s="38"/>
+      <c r="L59" s="38"/>
+      <c r="M59" s="38"/>
+      <c r="N59" s="38"/>
+      <c r="O59" s="38"/>
+      <c r="P59" s="38"/>
+      <c r="Q59" s="38"/>
+      <c r="R59" s="38"/>
+      <c r="S59" s="38"/>
+      <c r="T59" s="38"/>
+      <c r="U59" s="38"/>
+      <c r="V59" s="38"/>
+      <c r="W59" s="38"/>
+      <c r="X59" s="38"/>
+      <c r="Y59" s="38"/>
+      <c r="Z59" s="38"/>
+      <c r="AA59" s="38"/>
+      <c r="AB59" s="38"/>
+      <c r="AC59" s="38"/>
+      <c r="AD59" s="38"/>
+      <c r="AE59" s="38"/>
+      <c r="AF59" s="38"/>
+      <c r="AG59" s="38"/>
+      <c r="AH59" s="38"/>
+      <c r="AI59" s="38"/>
+      <c r="AJ59" s="38"/>
+      <c r="AK59" s="38"/>
+      <c r="AL59" s="38"/>
+      <c r="AM59" s="38"/>
+      <c r="AN59" s="38"/>
+      <c r="AO59" s="38"/>
+      <c r="AP59" s="38"/>
+      <c r="AQ59" s="38"/>
+      <c r="AR59" s="38"/>
+      <c r="AS59" s="38"/>
+      <c r="AT59" s="38"/>
+      <c r="AU59" s="38"/>
+      <c r="AV59" s="38"/>
+      <c r="AW59" s="38"/>
+      <c r="AX59" s="38"/>
+      <c r="AY59" s="38"/>
+      <c r="AZ59" s="38"/>
+      <c r="BA59" s="38"/>
+      <c r="BB59" s="38"/>
+      <c r="BC59" s="38"/>
+      <c r="BD59" s="38"/>
+      <c r="BE59" s="38"/>
+      <c r="BF59" s="38"/>
+      <c r="BG59" s="38"/>
+      <c r="BH59" s="38"/>
+      <c r="BI59" s="38"/>
+      <c r="BJ59" s="38"/>
+      <c r="BK59" s="38"/>
+      <c r="BL59" s="38"/>
+      <c r="BM59" s="38"/>
     </row>
-    <row r="60" spans="1:65" s="2" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:65" s="2" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
       <c r="B60" s="41"/>
       <c r="C60" s="53"/>
@@ -15649,77 +15504,245 @@
       <c r="BL60" s="38"/>
       <c r="BM60" s="38"/>
     </row>
-    <row r="61" spans="1:65" s="2" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+    <row r="61" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
       <c r="B61" s="41"/>
-      <c r="C61" s="53"/>
+      <c r="C61" s="41"/>
       <c r="D61" s="34"/>
       <c r="E61" s="34"/>
       <c r="F61" s="31"/>
       <c r="G61" s="32"/>
       <c r="H61" s="33"/>
       <c r="I61" s="26"/>
-      <c r="J61" s="38"/>
-      <c r="K61" s="38"/>
-      <c r="L61" s="38"/>
-      <c r="M61" s="38"/>
-      <c r="N61" s="38"/>
-      <c r="O61" s="38"/>
-      <c r="P61" s="38"/>
-      <c r="Q61" s="38"/>
-      <c r="R61" s="38"/>
-      <c r="S61" s="38"/>
-      <c r="T61" s="38"/>
-      <c r="U61" s="38"/>
-      <c r="V61" s="38"/>
-      <c r="W61" s="38"/>
-      <c r="X61" s="38"/>
-      <c r="Y61" s="38"/>
-      <c r="Z61" s="38"/>
-      <c r="AA61" s="38"/>
-      <c r="AB61" s="38"/>
-      <c r="AC61" s="38"/>
-      <c r="AD61" s="38"/>
-      <c r="AE61" s="38"/>
-      <c r="AF61" s="38"/>
-      <c r="AG61" s="38"/>
-      <c r="AH61" s="38"/>
-      <c r="AI61" s="38"/>
-      <c r="AJ61" s="38"/>
-      <c r="AK61" s="38"/>
-      <c r="AL61" s="38"/>
-      <c r="AM61" s="38"/>
-      <c r="AN61" s="38"/>
-      <c r="AO61" s="38"/>
-      <c r="AP61" s="38"/>
-      <c r="AQ61" s="38"/>
-      <c r="AR61" s="38"/>
-      <c r="AS61" s="38"/>
-      <c r="AT61" s="38"/>
-      <c r="AU61" s="38"/>
-      <c r="AV61" s="38"/>
-      <c r="AW61" s="38"/>
-      <c r="AX61" s="38"/>
-      <c r="AY61" s="38"/>
-      <c r="AZ61" s="38"/>
-      <c r="BA61" s="38"/>
-      <c r="BB61" s="38"/>
-      <c r="BC61" s="38"/>
-      <c r="BD61" s="38"/>
-      <c r="BE61" s="38"/>
-      <c r="BF61" s="38"/>
-      <c r="BG61" s="38"/>
-      <c r="BH61" s="38"/>
-      <c r="BI61" s="38"/>
-      <c r="BJ61" s="38"/>
-      <c r="BK61" s="38"/>
-      <c r="BL61" s="38"/>
-      <c r="BM61" s="38"/>
+      <c r="J61" s="38" t="str">
+        <f t="shared" ref="J61:S62" ca="1" si="26">IF(AND($D61="Goal",J$5&gt;=$G61,J$5&lt;=$G61+$H61-1),2,IF(AND($D61="Milestone",J$5&gt;=$G61,J$5&lt;=$G61+$H61-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="K61" s="38" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="L61" s="38" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="M61" s="38" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="N61" s="38" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="O61" s="38" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="P61" s="38" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="Q61" s="38" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="R61" s="38" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="S61" s="38" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="T61" s="38" t="str">
+        <f t="shared" ref="T61:AC62" ca="1" si="27">IF(AND($D61="Goal",T$5&gt;=$G61,T$5&lt;=$G61+$H61-1),2,IF(AND($D61="Milestone",T$5&gt;=$G61,T$5&lt;=$G61+$H61-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="U61" s="38" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v/>
+      </c>
+      <c r="V61" s="38" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v/>
+      </c>
+      <c r="W61" s="38" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v/>
+      </c>
+      <c r="X61" s="38" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v/>
+      </c>
+      <c r="Y61" s="38" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v/>
+      </c>
+      <c r="Z61" s="38" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v/>
+      </c>
+      <c r="AA61" s="38" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v/>
+      </c>
+      <c r="AB61" s="38" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v/>
+      </c>
+      <c r="AC61" s="38" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v/>
+      </c>
+      <c r="AD61" s="38" t="str">
+        <f t="shared" ref="AD61:AM62" ca="1" si="28">IF(AND($D61="Goal",AD$5&gt;=$G61,AD$5&lt;=$G61+$H61-1),2,IF(AND($D61="Milestone",AD$5&gt;=$G61,AD$5&lt;=$G61+$H61-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AE61" s="38" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AF61" s="38" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AG61" s="38" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AH61" s="38" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AI61" s="38" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AJ61" s="38" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AK61" s="38" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AL61" s="38" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AM61" s="38" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AN61" s="38" t="str">
+        <f t="shared" ref="AN61:AW62" ca="1" si="29">IF(AND($D61="Goal",AN$5&gt;=$G61,AN$5&lt;=$G61+$H61-1),2,IF(AND($D61="Milestone",AN$5&gt;=$G61,AN$5&lt;=$G61+$H61-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AO61" s="38" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AP61" s="38" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AQ61" s="38" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AR61" s="38" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AS61" s="38" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AT61" s="38" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AU61" s="38" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AV61" s="38" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AW61" s="38" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AX61" s="38" t="str">
+        <f t="shared" ref="AX61:BG62" ca="1" si="30">IF(AND($D61="Goal",AX$5&gt;=$G61,AX$5&lt;=$G61+$H61-1),2,IF(AND($D61="Milestone",AX$5&gt;=$G61,AX$5&lt;=$G61+$H61-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AY61" s="38" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="AZ61" s="38" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="BA61" s="38" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="BB61" s="38" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="BC61" s="38" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="BD61" s="38" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="BE61" s="38" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="BF61" s="38" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="BG61" s="38" t="str">
+        <f t="shared" ca="1" si="30"/>
+        <v/>
+      </c>
+      <c r="BH61" s="38" t="str">
+        <f t="shared" ref="BH61:BM62" ca="1" si="31">IF(AND($D61="Goal",BH$5&gt;=$G61,BH$5&lt;=$G61+$H61-1),2,IF(AND($D61="Milestone",BH$5&gt;=$G61,BH$5&lt;=$G61+$H61-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BI61" s="38" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="BJ61" s="38" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="BK61" s="38" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="BL61" s="38" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="BM61" s="38" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
     </row>
     <row r="62" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
       <c r="B62" s="41"/>
-      <c r="C62" s="41"/>
+      <c r="C62" s="53"/>
       <c r="D62" s="34"/>
       <c r="E62" s="34"/>
       <c r="F62" s="31"/>
@@ -15727,7 +15750,7 @@
       <c r="H62" s="33"/>
       <c r="I62" s="26"/>
       <c r="J62" s="38" t="str">
-        <f t="shared" ref="J62:S63" ca="1" si="26">IF(AND($D62="Goal",J$5&gt;=$G62,J$5&lt;=$G62+$H62-1),2,IF(AND($D62="Milestone",J$5&gt;=$G62,J$5&lt;=$G62+$H62-1),1,""))</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="K62" s="38" t="str">
@@ -15767,7 +15790,7 @@
         <v/>
       </c>
       <c r="T62" s="38" t="str">
-        <f t="shared" ref="T62:AC63" ca="1" si="27">IF(AND($D62="Goal",T$5&gt;=$G62,T$5&lt;=$G62+$H62-1),2,IF(AND($D62="Milestone",T$5&gt;=$G62,T$5&lt;=$G62+$H62-1),1,""))</f>
+        <f t="shared" ca="1" si="27"/>
         <v/>
       </c>
       <c r="U62" s="38" t="str">
@@ -15807,7 +15830,7 @@
         <v/>
       </c>
       <c r="AD62" s="38" t="str">
-        <f t="shared" ref="AD62:AM63" ca="1" si="28">IF(AND($D62="Goal",AD$5&gt;=$G62,AD$5&lt;=$G62+$H62-1),2,IF(AND($D62="Milestone",AD$5&gt;=$G62,AD$5&lt;=$G62+$H62-1),1,""))</f>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AE62" s="38" t="str">
@@ -15847,7 +15870,7 @@
         <v/>
       </c>
       <c r="AN62" s="38" t="str">
-        <f t="shared" ref="AN62:AW63" ca="1" si="29">IF(AND($D62="Goal",AN$5&gt;=$G62,AN$5&lt;=$G62+$H62-1),2,IF(AND($D62="Milestone",AN$5&gt;=$G62,AN$5&lt;=$G62+$H62-1),1,""))</f>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AO62" s="38" t="str">
@@ -15887,7 +15910,7 @@
         <v/>
       </c>
       <c r="AX62" s="38" t="str">
-        <f t="shared" ref="AX62:BG63" ca="1" si="30">IF(AND($D62="Goal",AX$5&gt;=$G62,AX$5&lt;=$G62+$H62-1),2,IF(AND($D62="Milestone",AX$5&gt;=$G62,AX$5&lt;=$G62+$H62-1),1,""))</f>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AY62" s="38" t="str">
@@ -15927,7 +15950,7 @@
         <v/>
       </c>
       <c r="BH62" s="38" t="str">
-        <f t="shared" ref="BH62:BM63" ca="1" si="31">IF(AND($D62="Goal",BH$5&gt;=$G62,BH$5&lt;=$G62+$H62-1),2,IF(AND($D62="Milestone",BH$5&gt;=$G62,BH$5&lt;=$G62+$H62-1),1,""))</f>
+        <f t="shared" ca="1" si="31"/>
         <v/>
       </c>
       <c r="BI62" s="38" t="str">
@@ -15962,234 +15985,234 @@
       <c r="H63" s="33"/>
       <c r="I63" s="26"/>
       <c r="J63" s="38" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ref="J63:S72" ca="1" si="32">IF(AND($D63="Goal",J$5&gt;=$G63,J$5&lt;=$G63+$H63-1),2,IF(AND($D63="Milestone",J$5&gt;=$G63,J$5&lt;=$G63+$H63-1),1,""))</f>
         <v/>
       </c>
       <c r="K63" s="38" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="L63" s="38" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="M63" s="38" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="N63" s="38" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="O63" s="38" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="P63" s="38" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="Q63" s="38" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="R63" s="38" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="S63" s="38" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="T63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ref="T63:AC72" ca="1" si="33">IF(AND($D63="Goal",T$5&gt;=$G63,T$5&lt;=$G63+$H63-1),2,IF(AND($D63="Milestone",T$5&gt;=$G63,T$5&lt;=$G63+$H63-1),1,""))</f>
         <v/>
       </c>
       <c r="U63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="V63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="W63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="X63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Y63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="Z63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AA63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AB63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AC63" s="38" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="AD63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ref="AD63:AM72" ca="1" si="34">IF(AND($D63="Goal",AD$5&gt;=$G63,AD$5&lt;=$G63+$H63-1),2,IF(AND($D63="Milestone",AD$5&gt;=$G63,AD$5&lt;=$G63+$H63-1),1,""))</f>
         <v/>
       </c>
       <c r="AE63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AF63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AG63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AH63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AI63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AJ63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AK63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AL63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AM63" s="38" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AN63" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ref="AN63:AW72" ca="1" si="35">IF(AND($D63="Goal",AN$5&gt;=$G63,AN$5&lt;=$G63+$H63-1),2,IF(AND($D63="Milestone",AN$5&gt;=$G63,AN$5&lt;=$G63+$H63-1),1,""))</f>
         <v/>
       </c>
       <c r="AO63" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AP63" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AQ63" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AR63" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AS63" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AT63" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AU63" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AV63" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AW63" s="38" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AX63" s="38" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ref="AX63:BG72" ca="1" si="36">IF(AND($D63="Goal",AX$5&gt;=$G63,AX$5&lt;=$G63+$H63-1),2,IF(AND($D63="Milestone",AX$5&gt;=$G63,AX$5&lt;=$G63+$H63-1),1,""))</f>
         <v/>
       </c>
       <c r="AY63" s="38" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="AZ63" s="38" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="BA63" s="38" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="BB63" s="38" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="BC63" s="38" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="BD63" s="38" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="BE63" s="38" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="BF63" s="38" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="BG63" s="38" t="str">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="BH63" s="38" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ref="BH63:BM72" ca="1" si="37">IF(AND($D63="Goal",BH$5&gt;=$G63,BH$5&lt;=$G63+$H63-1),2,IF(AND($D63="Milestone",BH$5&gt;=$G63,BH$5&lt;=$G63+$H63-1),1,""))</f>
         <v/>
       </c>
       <c r="BI63" s="38" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="BJ63" s="38" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="BK63" s="38" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="BL63" s="38" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="BM63" s="38" t="str">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" s="41"/>
-      <c r="C64" s="53"/>
+      <c r="C64" s="41"/>
       <c r="D64" s="34"/>
       <c r="E64" s="34"/>
       <c r="F64" s="31"/>
@@ -16197,7 +16220,7 @@
       <c r="H64" s="33"/>
       <c r="I64" s="26"/>
       <c r="J64" s="38" t="str">
-        <f t="shared" ref="J64:S72" ca="1" si="32">IF(AND($D64="Goal",J$5&gt;=$G64,J$5&lt;=$G64+$H64-1),2,IF(AND($D64="Milestone",J$5&gt;=$G64,J$5&lt;=$G64+$H64-1),1,""))</f>
+        <f t="shared" ca="1" si="32"/>
         <v/>
       </c>
       <c r="K64" s="38" t="str">
@@ -16237,7 +16260,7 @@
         <v/>
       </c>
       <c r="T64" s="38" t="str">
-        <f t="shared" ref="T64:AC72" ca="1" si="33">IF(AND($D64="Goal",T$5&gt;=$G64,T$5&lt;=$G64+$H64-1),2,IF(AND($D64="Milestone",T$5&gt;=$G64,T$5&lt;=$G64+$H64-1),1,""))</f>
+        <f t="shared" ca="1" si="33"/>
         <v/>
       </c>
       <c r="U64" s="38" t="str">
@@ -16277,7 +16300,7 @@
         <v/>
       </c>
       <c r="AD64" s="38" t="str">
-        <f t="shared" ref="AD64:AM72" ca="1" si="34">IF(AND($D64="Goal",AD$5&gt;=$G64,AD$5&lt;=$G64+$H64-1),2,IF(AND($D64="Milestone",AD$5&gt;=$G64,AD$5&lt;=$G64+$H64-1),1,""))</f>
+        <f t="shared" ca="1" si="34"/>
         <v/>
       </c>
       <c r="AE64" s="38" t="str">
@@ -16317,7 +16340,7 @@
         <v/>
       </c>
       <c r="AN64" s="38" t="str">
-        <f t="shared" ref="AN64:AW72" ca="1" si="35">IF(AND($D64="Goal",AN$5&gt;=$G64,AN$5&lt;=$G64+$H64-1),2,IF(AND($D64="Milestone",AN$5&gt;=$G64,AN$5&lt;=$G64+$H64-1),1,""))</f>
+        <f t="shared" ca="1" si="35"/>
         <v/>
       </c>
       <c r="AO64" s="38" t="str">
@@ -16357,7 +16380,7 @@
         <v/>
       </c>
       <c r="AX64" s="38" t="str">
-        <f t="shared" ref="AX64:BG72" ca="1" si="36">IF(AND($D64="Goal",AX$5&gt;=$G64,AX$5&lt;=$G64+$H64-1),2,IF(AND($D64="Milestone",AX$5&gt;=$G64,AX$5&lt;=$G64+$H64-1),1,""))</f>
+        <f t="shared" ca="1" si="36"/>
         <v/>
       </c>
       <c r="AY64" s="38" t="str">
@@ -16397,7 +16420,7 @@
         <v/>
       </c>
       <c r="BH64" s="38" t="str">
-        <f t="shared" ref="BH64:BM72" ca="1" si="37">IF(AND($D64="Goal",BH$5&gt;=$G64,BH$5&lt;=$G64+$H64-1),2,IF(AND($D64="Milestone",BH$5&gt;=$G64,BH$5&lt;=$G64+$H64-1),1,""))</f>
+        <f t="shared" ca="1" si="37"/>
         <v/>
       </c>
       <c r="BI64" s="38" t="str">
@@ -16423,7 +16446,9 @@
     </row>
     <row r="65" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14"/>
-      <c r="B65" s="41"/>
+      <c r="B65" s="53" t="s">
+        <v>50</v>
+      </c>
       <c r="C65" s="41"/>
       <c r="D65" s="34"/>
       <c r="E65" s="34"/>
@@ -16658,315 +16683,319 @@
     </row>
     <row r="66" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14"/>
-      <c r="B66" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="C66" s="41"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
+      <c r="B66" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C66" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="34">
+        <v>4</v>
+      </c>
       <c r="F66" s="31"/>
       <c r="G66" s="32"/>
       <c r="H66" s="33"/>
       <c r="I66" s="26"/>
-      <c r="J66" s="38" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-      <c r="K66" s="38" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-      <c r="L66" s="38" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-      <c r="M66" s="38" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-      <c r="N66" s="38" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-      <c r="O66" s="38" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-      <c r="P66" s="38" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-      <c r="Q66" s="38" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-      <c r="R66" s="38" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-      <c r="S66" s="38" t="str">
-        <f t="shared" ca="1" si="32"/>
-        <v/>
-      </c>
-      <c r="T66" s="38" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v/>
-      </c>
-      <c r="U66" s="38" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v/>
-      </c>
-      <c r="V66" s="38" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v/>
-      </c>
-      <c r="W66" s="38" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v/>
-      </c>
-      <c r="X66" s="38" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v/>
-      </c>
-      <c r="Y66" s="38" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v/>
-      </c>
-      <c r="Z66" s="38" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v/>
-      </c>
-      <c r="AA66" s="38" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v/>
-      </c>
-      <c r="AB66" s="38" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v/>
-      </c>
-      <c r="AC66" s="38" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v/>
-      </c>
-      <c r="AD66" s="38" t="str">
-        <f t="shared" ca="1" si="34"/>
-        <v/>
-      </c>
-      <c r="AE66" s="38" t="str">
-        <f t="shared" ca="1" si="34"/>
-        <v/>
-      </c>
-      <c r="AF66" s="38" t="str">
-        <f t="shared" ca="1" si="34"/>
-        <v/>
-      </c>
-      <c r="AG66" s="38" t="str">
-        <f t="shared" ca="1" si="34"/>
-        <v/>
-      </c>
-      <c r="AH66" s="38" t="str">
-        <f t="shared" ca="1" si="34"/>
-        <v/>
-      </c>
-      <c r="AI66" s="38" t="str">
-        <f t="shared" ca="1" si="34"/>
-        <v/>
-      </c>
-      <c r="AJ66" s="38" t="str">
-        <f t="shared" ca="1" si="34"/>
-        <v/>
-      </c>
-      <c r="AK66" s="38" t="str">
-        <f t="shared" ca="1" si="34"/>
-        <v/>
-      </c>
-      <c r="AL66" s="38" t="str">
-        <f t="shared" ca="1" si="34"/>
-        <v/>
-      </c>
-      <c r="AM66" s="38" t="str">
-        <f t="shared" ca="1" si="34"/>
-        <v/>
-      </c>
-      <c r="AN66" s="38" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v/>
-      </c>
-      <c r="AO66" s="38" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v/>
-      </c>
-      <c r="AP66" s="38" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v/>
-      </c>
-      <c r="AQ66" s="38" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v/>
-      </c>
-      <c r="AR66" s="38" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v/>
-      </c>
-      <c r="AS66" s="38" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v/>
-      </c>
-      <c r="AT66" s="38" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v/>
-      </c>
-      <c r="AU66" s="38" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v/>
-      </c>
-      <c r="AV66" s="38" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v/>
-      </c>
-      <c r="AW66" s="38" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v/>
-      </c>
-      <c r="AX66" s="38" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v/>
-      </c>
-      <c r="AY66" s="38" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v/>
-      </c>
-      <c r="AZ66" s="38" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v/>
-      </c>
-      <c r="BA66" s="38" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v/>
-      </c>
-      <c r="BB66" s="38" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v/>
-      </c>
-      <c r="BC66" s="38" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v/>
-      </c>
-      <c r="BD66" s="38" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v/>
-      </c>
-      <c r="BE66" s="38" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v/>
-      </c>
-      <c r="BF66" s="38" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v/>
-      </c>
-      <c r="BG66" s="38" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v/>
-      </c>
-      <c r="BH66" s="38" t="str">
-        <f t="shared" ca="1" si="37"/>
-        <v/>
-      </c>
-      <c r="BI66" s="38" t="str">
-        <f t="shared" ca="1" si="37"/>
-        <v/>
-      </c>
-      <c r="BJ66" s="38" t="str">
-        <f t="shared" ca="1" si="37"/>
-        <v/>
-      </c>
-      <c r="BK66" s="38" t="str">
-        <f t="shared" ca="1" si="37"/>
-        <v/>
-      </c>
-      <c r="BL66" s="38" t="str">
-        <f t="shared" ca="1" si="37"/>
-        <v/>
-      </c>
-      <c r="BM66" s="38" t="str">
-        <f t="shared" ca="1" si="37"/>
-        <v/>
-      </c>
+      <c r="J66" s="38"/>
+      <c r="K66" s="38"/>
+      <c r="L66" s="38"/>
+      <c r="M66" s="38"/>
+      <c r="N66" s="38"/>
+      <c r="O66" s="38"/>
+      <c r="P66" s="38"/>
+      <c r="Q66" s="38"/>
+      <c r="R66" s="38"/>
+      <c r="S66" s="38"/>
+      <c r="T66" s="38"/>
+      <c r="U66" s="38"/>
+      <c r="V66" s="38"/>
+      <c r="W66" s="38"/>
+      <c r="X66" s="38"/>
+      <c r="Y66" s="38"/>
+      <c r="Z66" s="38"/>
+      <c r="AA66" s="38"/>
+      <c r="AB66" s="38"/>
+      <c r="AC66" s="38"/>
+      <c r="AD66" s="38"/>
+      <c r="AE66" s="38"/>
+      <c r="AF66" s="38"/>
+      <c r="AG66" s="38"/>
+      <c r="AH66" s="38"/>
+      <c r="AI66" s="38"/>
+      <c r="AJ66" s="38"/>
+      <c r="AK66" s="38"/>
+      <c r="AL66" s="38"/>
+      <c r="AM66" s="38"/>
+      <c r="AN66" s="38"/>
+      <c r="AO66" s="38"/>
+      <c r="AP66" s="38"/>
+      <c r="AQ66" s="38"/>
+      <c r="AR66" s="38"/>
+      <c r="AS66" s="38"/>
+      <c r="AT66" s="38"/>
+      <c r="AU66" s="38"/>
+      <c r="AV66" s="38"/>
+      <c r="AW66" s="38"/>
+      <c r="AX66" s="38"/>
+      <c r="AY66" s="38"/>
+      <c r="AZ66" s="38"/>
+      <c r="BA66" s="38"/>
+      <c r="BB66" s="38"/>
+      <c r="BC66" s="38"/>
+      <c r="BD66" s="38"/>
+      <c r="BE66" s="38"/>
+      <c r="BF66" s="38"/>
+      <c r="BG66" s="38"/>
+      <c r="BH66" s="38"/>
+      <c r="BI66" s="38"/>
+      <c r="BJ66" s="38"/>
+      <c r="BK66" s="38"/>
+      <c r="BL66" s="38"/>
+      <c r="BM66" s="38"/>
     </row>
     <row r="67" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
-      <c r="B67" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="C67" s="41" t="s">
-        <v>63</v>
-      </c>
+      <c r="B67" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C67" s="53"/>
       <c r="D67" s="34" t="s">
         <v>17</v>
       </c>
       <c r="E67" s="34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F67" s="31"/>
       <c r="G67" s="32"/>
       <c r="H67" s="33"/>
       <c r="I67" s="26"/>
-      <c r="J67" s="38"/>
-      <c r="K67" s="38"/>
-      <c r="L67" s="38"/>
-      <c r="M67" s="38"/>
-      <c r="N67" s="38"/>
-      <c r="O67" s="38"/>
-      <c r="P67" s="38"/>
-      <c r="Q67" s="38"/>
-      <c r="R67" s="38"/>
-      <c r="S67" s="38"/>
-      <c r="T67" s="38"/>
-      <c r="U67" s="38"/>
-      <c r="V67" s="38"/>
-      <c r="W67" s="38"/>
-      <c r="X67" s="38"/>
-      <c r="Y67" s="38"/>
-      <c r="Z67" s="38"/>
-      <c r="AA67" s="38"/>
-      <c r="AB67" s="38"/>
-      <c r="AC67" s="38"/>
-      <c r="AD67" s="38"/>
-      <c r="AE67" s="38"/>
-      <c r="AF67" s="38"/>
-      <c r="AG67" s="38"/>
-      <c r="AH67" s="38"/>
-      <c r="AI67" s="38"/>
-      <c r="AJ67" s="38"/>
-      <c r="AK67" s="38"/>
-      <c r="AL67" s="38"/>
-      <c r="AM67" s="38"/>
-      <c r="AN67" s="38"/>
-      <c r="AO67" s="38"/>
-      <c r="AP67" s="38"/>
-      <c r="AQ67" s="38"/>
-      <c r="AR67" s="38"/>
-      <c r="AS67" s="38"/>
-      <c r="AT67" s="38"/>
-      <c r="AU67" s="38"/>
-      <c r="AV67" s="38"/>
-      <c r="AW67" s="38"/>
-      <c r="AX67" s="38"/>
-      <c r="AY67" s="38"/>
-      <c r="AZ67" s="38"/>
-      <c r="BA67" s="38"/>
-      <c r="BB67" s="38"/>
-      <c r="BC67" s="38"/>
-      <c r="BD67" s="38"/>
-      <c r="BE67" s="38"/>
-      <c r="BF67" s="38"/>
-      <c r="BG67" s="38"/>
-      <c r="BH67" s="38"/>
-      <c r="BI67" s="38"/>
-      <c r="BJ67" s="38"/>
-      <c r="BK67" s="38"/>
-      <c r="BL67" s="38"/>
-      <c r="BM67" s="38"/>
+      <c r="J67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",J$5&gt;=$G67,J$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",J$5&gt;=$G67,J$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="K67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",K$5&gt;=$G67,K$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",K$5&gt;=$G67,K$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="L67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",L$5&gt;=$G67,L$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",L$5&gt;=$G67,L$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="M67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",M$5&gt;=$G67,M$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",M$5&gt;=$G67,M$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="N67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",N$5&gt;=$G67,N$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",N$5&gt;=$G67,N$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="O67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",O$5&gt;=$G67,O$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",O$5&gt;=$G67,O$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="P67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",P$5&gt;=$G67,P$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",P$5&gt;=$G67,P$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="Q67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",Q$5&gt;=$G67,Q$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",Q$5&gt;=$G67,Q$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="R67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",R$5&gt;=$G67,R$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",R$5&gt;=$G67,R$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="S67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",S$5&gt;=$G67,S$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",S$5&gt;=$G67,S$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="T67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",T$5&gt;=$G67,T$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",T$5&gt;=$G67,T$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="U67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",U$5&gt;=$G67,U$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",U$5&gt;=$G67,U$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="V67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",V$5&gt;=$G67,V$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",V$5&gt;=$G67,V$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="W67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",W$5&gt;=$G67,W$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",W$5&gt;=$G67,W$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="X67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",X$5&gt;=$G67,X$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",X$5&gt;=$G67,X$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="Y67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",Y$5&gt;=$G67,Y$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",Y$5&gt;=$G67,Y$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="Z67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",Z$5&gt;=$G67,Z$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",Z$5&gt;=$G67,Z$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AA67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AA$5&gt;=$G67,AA$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AA$5&gt;=$G67,AA$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AB67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AB$5&gt;=$G67,AB$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AB$5&gt;=$G67,AB$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AC67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AC$5&gt;=$G67,AC$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AC$5&gt;=$G67,AC$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AD67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AD$5&gt;=$G67,AD$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AD$5&gt;=$G67,AD$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AE67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AE$5&gt;=$G67,AE$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AE$5&gt;=$G67,AE$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AF67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AF$5&gt;=$G67,AF$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AF$5&gt;=$G67,AF$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AG67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AG$5&gt;=$G67,AG$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AG$5&gt;=$G67,AG$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AH67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AH$5&gt;=$G67,AH$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AH$5&gt;=$G67,AH$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AI67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AI$5&gt;=$G67,AI$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AI$5&gt;=$G67,AI$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AJ67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AJ$5&gt;=$G67,AJ$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AJ$5&gt;=$G67,AJ$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AK67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AK$5&gt;=$G67,AK$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AK$5&gt;=$G67,AK$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AL67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AL$5&gt;=$G67,AL$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AL$5&gt;=$G67,AL$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AM67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AM$5&gt;=$G67,AM$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AM$5&gt;=$G67,AM$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AN67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AN$5&gt;=$G67,AN$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AN$5&gt;=$G67,AN$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AO67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AO$5&gt;=$G67,AO$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AO$5&gt;=$G67,AO$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AP67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AP$5&gt;=$G67,AP$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AP$5&gt;=$G67,AP$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AQ67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AQ$5&gt;=$G67,AQ$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AQ$5&gt;=$G67,AQ$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AR67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AR$5&gt;=$G67,AR$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AR$5&gt;=$G67,AR$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AS67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AS$5&gt;=$G67,AS$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AS$5&gt;=$G67,AS$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AT67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AT$5&gt;=$G67,AT$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AT$5&gt;=$G67,AT$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AU67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AU$5&gt;=$G67,AU$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AU$5&gt;=$G67,AU$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AV67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AV$5&gt;=$G67,AV$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AV$5&gt;=$G67,AV$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AW67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AW$5&gt;=$G67,AW$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AW$5&gt;=$G67,AW$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AX67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AX$5&gt;=$G67,AX$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AX$5&gt;=$G67,AX$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AY67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AY$5&gt;=$G67,AY$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AY$5&gt;=$G67,AY$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AZ67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",AZ$5&gt;=$G67,AZ$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",AZ$5&gt;=$G67,AZ$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BA67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BA$5&gt;=$G67,BA$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BA$5&gt;=$G67,BA$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BB67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BB$5&gt;=$G67,BB$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BB$5&gt;=$G67,BB$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BC67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BC$5&gt;=$G67,BC$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BC$5&gt;=$G67,BC$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BD67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BD$5&gt;=$G67,BD$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BD$5&gt;=$G67,BD$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BE67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BE$5&gt;=$G67,BE$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BE$5&gt;=$G67,BE$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BF67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BF$5&gt;=$G67,BF$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BF$5&gt;=$G67,BF$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BG67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BG$5&gt;=$G67,BG$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BG$5&gt;=$G67,BG$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BH67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BH$5&gt;=$G67,BH$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BH$5&gt;=$G67,BH$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BI67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BI$5&gt;=$G67,BI$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BI$5&gt;=$G67,BI$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BJ67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BJ$5&gt;=$G67,BJ$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BJ$5&gt;=$G67,BJ$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BK67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BK$5&gt;=$G67,BK$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BK$5&gt;=$G67,BK$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BL67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BL$5&gt;=$G67,BL$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BL$5&gt;=$G67,BL$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BM67" s="38" t="str">
+        <f ca="1">IF(AND($D67="Goal",BM$5&gt;=$G67,BM$5&lt;=$G67+$H67-1),2,IF(AND($D67="Milestone",BM$5&gt;=$G67,BM$5&lt;=$G67+$H67-1),1,""))</f>
+        <v/>
+      </c>
     </row>
     <row r="68" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14"/>
@@ -18173,8 +18202,8 @@
       <c r="C75" s="41"/>
       <c r="D75" s="34"/>
       <c r="E75" s="34">
-        <f>SUBTOTAL(109,E67:E74)</f>
-        <v>31.5</v>
+        <f>SUBTOTAL(109,E66:E74)</f>
+        <v>33.5</v>
       </c>
       <c r="F75" s="31"/>
       <c r="G75" s="32"/>
@@ -27087,7 +27116,7 @@
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="T2:W2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F7:F8 F116 F88:F91 F97 F72:F73 F94 F103 F83:F86 F75:F76 F10 F62:F69 F22:F43 F45:F46 F53:F59 F50:F51 F48">
+  <conditionalFormatting sqref="F7:F8 F116 F88:F91 F97 F72:F73 F94 F103 F83:F86 F75:F76 F10 F22:F43 F45:F46 F52:F58 F49:F50 F61:F69">
     <cfRule type="dataBar" priority="254">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -27101,57 +27130,57 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5:BM8 J116:BM117 J88:BM91 J97:BM97 J72:BM73 J94:BM94 J103:BM103 J83:BM86 J75:BM76 J10:BM10 J62:BM69 J22:BM59">
-    <cfRule type="expression" dxfId="79" priority="247">
+  <conditionalFormatting sqref="J5:BM8 J116:BM117 J88:BM91 J97:BM97 J72:BM73 J94:BM94 J103:BM103 J83:BM86 J75:BM76 J10:BM10 J22:BM58 J61:BM69">
+    <cfRule type="expression" dxfId="75" priority="247">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:AN4">
-    <cfRule type="expression" dxfId="78" priority="253">
+    <cfRule type="expression" dxfId="74" priority="253">
       <formula>J$5&lt;=EOMONTH($J$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:BM4">
-    <cfRule type="expression" dxfId="77" priority="249">
+    <cfRule type="expression" dxfId="73" priority="249">
       <formula>AND(K$5&lt;=EOMONTH($J$5,2),K$5&gt;EOMONTH($J$5,0),K$5&gt;EOMONTH($J$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BM4">
-    <cfRule type="expression" dxfId="76" priority="248">
+    <cfRule type="expression" dxfId="72" priority="248">
       <formula>AND(J$5&lt;=EOMONTH($J$5,1),J$5&gt;EOMONTH($J$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:BM8 J10:BM10 J22:BM116">
-    <cfRule type="expression" dxfId="75" priority="270" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="270" stopIfTrue="1">
       <formula>AND($D8="Low risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="289" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="289" stopIfTrue="1">
       <formula>AND($D8="High risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="307" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="307" stopIfTrue="1">
       <formula>AND($D8="On track",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="308" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="308" stopIfTrue="1">
       <formula>AND($D8="Med risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="309" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="309" stopIfTrue="1">
       <formula>AND(LEN($D8)=0,J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J117:BM117">
-    <cfRule type="expression" dxfId="70" priority="317" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="317" stopIfTrue="1">
       <formula>AND(#REF!="Low risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="318" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="318" stopIfTrue="1">
       <formula>AND(#REF!="High risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="319" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="319" stopIfTrue="1">
       <formula>AND(#REF!="On track",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="320" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="320" stopIfTrue="1">
       <formula>AND(#REF!="Med risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="321" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="321" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27170,24 +27199,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="65" priority="238">
+    <cfRule type="expression" dxfId="61" priority="238">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="64" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="240" stopIfTrue="1">
       <formula>AND($D9="Low risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="241" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="241" stopIfTrue="1">
       <formula>AND($D9="High risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="242" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="242" stopIfTrue="1">
       <formula>AND($D9="On track",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="243" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="243" stopIfTrue="1">
       <formula>AND($D9="Med risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="244" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="244" stopIfTrue="1">
       <formula>AND(LEN($D9)=0,J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27206,7 +27235,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J80:BM80 J77:BM78">
-    <cfRule type="expression" dxfId="59" priority="222">
+    <cfRule type="expression" dxfId="55" priority="222">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27225,11 +27254,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J82:GC82">
-    <cfRule type="expression" dxfId="58" priority="213">
+    <cfRule type="expression" dxfId="54" priority="213">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F81 F79">
+  <conditionalFormatting sqref="F79 F81">
     <cfRule type="dataBar" priority="205">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -27244,11 +27273,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:BM81 J79:BM79">
-    <cfRule type="expression" dxfId="57" priority="206">
+    <cfRule type="expression" dxfId="53" priority="206">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F60:F61">
+  <conditionalFormatting sqref="F59:F60">
     <cfRule type="dataBar" priority="197">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -27262,8 +27291,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J60:BM61">
-    <cfRule type="expression" dxfId="56" priority="198">
+  <conditionalFormatting sqref="J59:BM60">
+    <cfRule type="expression" dxfId="52" priority="198">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27282,7 +27311,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87:GC87">
-    <cfRule type="expression" dxfId="55" priority="189">
+    <cfRule type="expression" dxfId="51" priority="189">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27301,7 +27330,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J98:GC99 J101:GC103 J106:GC106 J113:GC115">
-    <cfRule type="expression" dxfId="54" priority="182">
+    <cfRule type="expression" dxfId="50" priority="182">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27320,7 +27349,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:GC100">
-    <cfRule type="expression" dxfId="53" priority="174">
+    <cfRule type="expression" dxfId="49" priority="174">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27339,7 +27368,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J96:GC96">
-    <cfRule type="expression" dxfId="52" priority="165">
+    <cfRule type="expression" dxfId="48" priority="165">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27358,7 +27387,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J71:GC71">
-    <cfRule type="expression" dxfId="51" priority="157">
+    <cfRule type="expression" dxfId="47" priority="157">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27377,7 +27406,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J93:BM93">
-    <cfRule type="expression" dxfId="50" priority="149">
+    <cfRule type="expression" dxfId="46" priority="149">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27396,7 +27425,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J104:GC105">
-    <cfRule type="expression" dxfId="49" priority="141">
+    <cfRule type="expression" dxfId="45" priority="141">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27415,7 +27444,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J107:GC108">
-    <cfRule type="expression" dxfId="48" priority="133">
+    <cfRule type="expression" dxfId="44" priority="133">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27434,7 +27463,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J111:GC111">
-    <cfRule type="expression" dxfId="47" priority="125">
+    <cfRule type="expression" dxfId="43" priority="125">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27453,7 +27482,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J112:GC112">
-    <cfRule type="expression" dxfId="46" priority="117">
+    <cfRule type="expression" dxfId="42" priority="117">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27472,7 +27501,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J95:BM95">
-    <cfRule type="expression" dxfId="45" priority="109">
+    <cfRule type="expression" dxfId="41" priority="109">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27491,7 +27520,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J74:BM74">
-    <cfRule type="expression" dxfId="44" priority="101">
+    <cfRule type="expression" dxfId="40" priority="101">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27510,7 +27539,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J110:BM110">
-    <cfRule type="expression" dxfId="43" priority="93">
+    <cfRule type="expression" dxfId="39" priority="93">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27529,7 +27558,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J92:BM92">
-    <cfRule type="expression" dxfId="42" priority="61">
+    <cfRule type="expression" dxfId="38" priority="61">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27548,12 +27577,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:GC109">
-    <cfRule type="expression" dxfId="41" priority="69">
+    <cfRule type="expression" dxfId="37" priority="69">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70:BM70">
-    <cfRule type="expression" dxfId="40" priority="53">
+    <cfRule type="expression" dxfId="36" priority="53">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27586,24 +27615,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="39" priority="45">
+    <cfRule type="expression" dxfId="35" priority="45">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="38" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="47" stopIfTrue="1">
       <formula>AND($D11="Low risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="48" stopIfTrue="1">
       <formula>AND($D11="High risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="49" stopIfTrue="1">
       <formula>AND($D11="On track",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="50" stopIfTrue="1">
       <formula>AND($D11="Med risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="51" stopIfTrue="1">
       <formula>AND(LEN($D11)=0,J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27622,24 +27651,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="33" priority="37">
+    <cfRule type="expression" dxfId="29" priority="37">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="32" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="39" stopIfTrue="1">
       <formula>AND($D12="Low risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="40" stopIfTrue="1">
       <formula>AND($D12="High risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="41" stopIfTrue="1">
       <formula>AND($D12="On track",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="42" stopIfTrue="1">
       <formula>AND($D12="Med risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="43" stopIfTrue="1">
       <formula>AND(LEN($D12)=0,J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27658,24 +27687,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="27" priority="29">
+    <cfRule type="expression" dxfId="23" priority="29">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="26" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="31" stopIfTrue="1">
       <formula>AND($D15="Low risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="32" stopIfTrue="1">
       <formula>AND($D15="High risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="33" stopIfTrue="1">
       <formula>AND($D15="On track",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="34" stopIfTrue="1">
       <formula>AND($D15="Med risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="35" stopIfTrue="1">
       <formula>AND(LEN($D15)=0,J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27694,46 +27723,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="21" priority="21">
+    <cfRule type="expression" dxfId="17" priority="21">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="23" stopIfTrue="1">
       <formula>AND($D16="Low risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="24" stopIfTrue="1">
       <formula>AND($D16="High risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="25" stopIfTrue="1">
       <formula>AND($D16="On track",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="26" stopIfTrue="1">
       <formula>AND($D16="Med risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="27" stopIfTrue="1">
       <formula>AND(LEN($D16)=0,J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="16" stopIfTrue="1">
       <formula>AND($D19="Low risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="17" stopIfTrue="1">
       <formula>AND($D19="High risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="18" stopIfTrue="1">
       <formula>AND($D19="On track",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="19" stopIfTrue="1">
       <formula>AND($D19="Med risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="20" stopIfTrue="1">
       <formula>AND(LEN($D19)=0,J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="10" priority="13">
+    <cfRule type="expression" dxfId="6" priority="13">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27752,19 +27781,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:BM21">
-    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
       <formula>AND($D20="Low risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="9" stopIfTrue="1">
       <formula>AND($D20="High risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="10" stopIfTrue="1">
       <formula>AND($D20="On track",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="11" stopIfTrue="1">
       <formula>AND($D20="Med risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="12" stopIfTrue="1">
       <formula>AND(LEN($D20)=0,J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27783,7 +27812,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:GC21">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27801,7 +27830,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F52">
+  <conditionalFormatting sqref="F51">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -27815,7 +27844,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
+  <conditionalFormatting sqref="F48">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -27847,10 +27876,10 @@
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="G4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9 D11:D24 D60:D116" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9 D11:D24 D59:D116" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Goal,Milestone,On track, Low risk, Med risk, High risk"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D10 D22:D59" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D10 D67 D22:D47 D48:D58" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Goal,Milestone,On track, Low risk, Med risk, High risk"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27905,7 +27934,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F7:F8 F116 F88:F91 F97 F72:F73 F94 F103 F83:F86 F75:F76 F10 F62:F69 F22:F43 F45:F46 F53:F59 F50:F51 F48</xm:sqref>
+          <xm:sqref>F7:F8 F116 F88:F91 F97 F72:F73 F94 F103 F83:F86 F75:F76 F10 F22:F43 F45:F46 F52:F58 F49:F50 F61:F69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{AB15B3D1-2A05-48F7-BD43-B741E186FE95}">
@@ -27965,7 +27994,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F81 F79</xm:sqref>
+          <xm:sqref>F79 F81</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{20AD0325-5A08-4704-8CC7-A6E9457B1E3F}">
@@ -27980,7 +28009,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F60:F61</xm:sqref>
+          <xm:sqref>F59:F60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FB79D9D5-2573-4918-A758-531107DFB641}">
@@ -28340,7 +28369,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F52</xm:sqref>
+          <xm:sqref>F51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BDF1EDAE-75A8-4A38-9730-5006E07D0D5D}">
@@ -28355,7 +28384,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F49</xm:sqref>
+          <xm:sqref>F48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{DB5DC438-E855-400C-8FB0-BE37FFB333E9}">
@@ -28484,7 +28513,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>J60:BM61</xm:sqref>
+          <xm:sqref>J59:BM60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="379" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
@@ -28503,7 +28532,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>J116:BM116 J103:BM103 J8:BM8 J62:BM69 J88:BM91 J97:BM97 J72:BM73 J94:BM94 J83:BM86 J75:BM76 J10:BM10 J22:BM59</xm:sqref>
+          <xm:sqref>J116:BM116 J103:BM103 J8:BM8 J88:BM91 J97:BM97 J72:BM73 J94:BM94 J83:BM86 J75:BM76 J10:BM10 J22:BM58 J61:BM69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="196" id="{085A3FF5-1243-45B7-A70C-D34452A2D8D7}">

</xml_diff>